<commit_message>
improve courses_excel_parse run time
</commit_message>
<xml_diff>
--- a/courses.xlsx
+++ b/courses.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8250" activeTab="1"/>
+    <workbookView windowWidth="20385" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="students" sheetId="1" r:id="rId1"/>
     <sheet name="time" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">time!$A$1:$C$485</definedName>
+  </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
@@ -1486,12 +1489,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1501,7 +1504,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1522,23 +1525,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1546,25 +1534,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
       <color theme="3"/>
       <name val="等线"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1584,8 +1556,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1599,18 +1609,19 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1621,9 +1632,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1631,21 +1641,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1660,7 +1656,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1672,7 +1668,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1684,19 +1794,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1708,139 +1830,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1857,53 +1853,17 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1934,6 +1894,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1943,161 +1933,71 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="5"/>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="5"/>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3"/>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="8"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="4"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="6"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2424,7 +2324,7 @@
   <sheetPr/>
   <dimension ref="A1:C485"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -7771,9 +7671,6 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C485">
-    <sortCondition ref="C1"/>
-  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -7784,8 +7681,8 @@
   <sheetPr/>
   <dimension ref="A1:C485"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16" outlineLevelCol="2"/>
@@ -7795,7 +7692,7 @@
     <col min="3" max="3" width="20.3333333333333" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" ht="17.25" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7806,7 +7703,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" ht="17.25" spans="1:3">
       <c r="A2" s="2">
         <v>42561.3916666667</v>
       </c>
@@ -8488,7 +8385,7 @@
         <v>2163</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" ht="17.25" spans="1:3">
       <c r="A64" s="2">
         <v>42214.6368055556</v>
       </c>
@@ -8499,7 +8396,7 @@
         <v>2166</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" ht="17.25" spans="1:3">
       <c r="A65" s="2">
         <v>42569.7381944444</v>
       </c>
@@ -8510,7 +8407,7 @@
         <v>2241</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" ht="17.25" spans="1:3">
       <c r="A66" s="2">
         <v>42577.6770833333</v>
       </c>
@@ -13119,7 +13016,7 @@
         <v>5073894</v>
       </c>
     </row>
-    <row r="485" spans="1:3">
+    <row r="485" ht="17.25" spans="1:3">
       <c r="A485" s="2">
         <v>41407.4548611111</v>
       </c>
@@ -13131,9 +13028,6 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C485">
-    <sortCondition ref="C1"/>
-  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>

</xml_diff>